<commit_message>
Update Indian Liver Patient Dataset (ILPD).xlsx
</commit_message>
<xml_diff>
--- a/Indian Liver Patient Dataset (ILPD).xlsx
+++ b/Indian Liver Patient Dataset (ILPD).xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\GitHub\Datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C05CA38F-10D3-40A7-9907-EC623ADC8DB5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A92AADD-E3C0-4E58-9BB5-E6C4F089DAAB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-9900" yWindow="3264" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Indian Liver Patient Dataset (I" sheetId="1" r:id="rId1"/>
+    <sheet name="Indian Liver Patient Dataset" sheetId="1" r:id="rId1"/>
     <sheet name="Description" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Indian Liver Patient Dataset (I'!$A$1:$K$584</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Indian Liver Patient Dataset'!$A$1:$K$584</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -101,9 +101,6 @@
     <t>ALB</t>
   </si>
   <si>
-    <t>AG Ratio</t>
-  </si>
-  <si>
     <t>Class</t>
   </si>
   <si>
@@ -111,6 +108,9 @@
   </si>
   <si>
     <t>10. A/G Ratio Albumin and Globulin Ratio (has 4 missing values)</t>
+  </si>
+  <si>
+    <t>AG_Ratio</t>
   </si>
 </sst>
 </file>
@@ -968,8 +968,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K584"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1003,10 +1003,10 @@
         <v>24</v>
       </c>
       <c r="J1" t="s">
+        <v>28</v>
+      </c>
+      <c r="K1" t="s">
         <v>25</v>
-      </c>
-      <c r="K1" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
@@ -21412,7 +21412,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C75D704-E3E3-450B-9074-4A76F784AC80}">
   <dimension ref="A1:A19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
@@ -21490,12 +21490,12 @@
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>